<commit_message>
Fixed curl command to download license files
</commit_message>
<xml_diff>
--- a/tb-oss/Open Source Compliance Worksheet.xlsx
+++ b/tb-oss/Open Source Compliance Worksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\terraform\tranquilityBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orme\tranquility-base\tb-oss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29ABD8C7-D99C-4B9E-9988-8FD3F4CDD31A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D441D2B-5DC7-4C2B-8F4E-E3D62E023BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3825" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -724,13 +724,13 @@
     <t>Terraform Binary is downloaded and executed outside the image - do we need to worry about transitive deps coming from terrafrom ?</t>
   </si>
   <si>
-    <t>Likewise for nodeJS and Angular ?</t>
-  </si>
-  <si>
     <t>License download</t>
   </si>
   <si>
     <t>Need source code</t>
+  </si>
+  <si>
+    <t>Likewise for nodeJS and Angular?</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1225,6 +1225,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1285,10 +1290,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1683,20 +1684,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:26" ht="32.25" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="60"/>
+      <c r="B3" s="63"/>
     </row>
     <row r="4" spans="1:26" ht="45" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1723,10 +1724,10 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="32.25" customHeight="1">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="58"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1753,10 +1754,10 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="56"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1787,10 +1788,10 @@
       <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="36" customHeight="1">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="58"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1817,19 +1818,19 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="84" customHeight="1">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="56"/>
+      <c r="B9" s="59"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="28.5" customHeight="1">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="60"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1985,10 +1986,10 @@
       <c r="B23" s="33"/>
     </row>
     <row r="24" spans="1:26" ht="37.5" customHeight="1">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="62"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -3030,8 +3031,8 @@
   </sheetPr>
   <dimension ref="A1:AB996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="107" workbookViewId="0">
-      <selection activeCell="H47" sqref="H5:H47"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3079,13 +3080,13 @@
       <c r="AB1" s="14"/>
     </row>
     <row r="2" spans="1:28" ht="49.5" customHeight="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="56"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="59"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -3139,11 +3140,11 @@
       <c r="F4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="81" t="s">
-        <v>178</v>
-      </c>
-      <c r="H4" s="81" t="s">
+      <c r="G4" s="56" t="s">
         <v>177</v>
+      </c>
+      <c r="H4" s="56" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:28" s="37" customFormat="1" ht="15.75" customHeight="1">
@@ -3163,12 +3164,12 @@
       <c r="F5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B5," --output ",SUBSTITUTE(A5," ","-"),"-",IF((LEN(B5)-FIND("@",SUBSTITUTE(B5,"/","@",LEN(B5)-LEN(SUBSTITUTE(B5,"/",""))),1))&gt;0,RIGHT(B5,(LEN(B5)-FIND("@",SUBSTITUTE(B5,"/","@",LEN(B5)-LEN(SUBSTITUTE(B5,"/",""))),1))),SUBSTITUTE(RIGHT(B5,(LEN(B5)-FIND("@",SUBSTITUTE(B5,"/","@",LEN(B5)-LEN(SUBSTITUTE(B5,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/certifi/python-certifi/blob/master/LICENSE --output certifi-LICENSE</v>
+      <c r="H5" s="55" t="str">
+        <f t="shared" ref="H5:H46" si="0">_xlfn.CONCAT("curl ",SUBSTITUTE(SUBSTITUTE(B5,"github.com","raw.githubusercontent.com"),"/blob","")," --output ",SUBSTITUTE(A5," ","-"),"-",IF((LEN(B5)-FIND("@",SUBSTITUTE(B5,"/","@",LEN(B5)-LEN(SUBSTITUTE(B5,"/",""))),1))&gt;0,RIGHT(B5,(LEN(B5)-FIND("@",SUBSTITUTE(B5,"/","@",LEN(B5)-LEN(SUBSTITUTE(B5,"/",""))),1))),SUBSTITUTE(RIGHT(B5,(LEN(B5)-FIND("@",SUBSTITUTE(B5,"/","@",LEN(B5)-LEN(SUBSTITUTE(B5,"/",""))-1),1))),"/","")))</f>
+        <v>curl https://raw.githubusercontent.com/certifi/python-certifi/master/LICENSE --output certifi-LICENSE</v>
       </c>
     </row>
     <row r="6" spans="1:28" s="37" customFormat="1" ht="15.75" customHeight="1">
@@ -3188,12 +3189,12 @@
       <c r="F6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="82" t="s">
+      <c r="G6" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B6," --output ",SUBSTITUTE(A6," ","-"),"-",IF((LEN(B6)-FIND("@",SUBSTITUTE(B6,"/","@",LEN(B6)-LEN(SUBSTITUTE(B6,"/",""))),1))&gt;0,RIGHT(B6,(LEN(B6)-FIND("@",SUBSTITUTE(B6,"/","@",LEN(B6)-LEN(SUBSTITUTE(B6,"/",""))),1))),SUBSTITUTE(RIGHT(B6,(LEN(B6)-FIND("@",SUBSTITUTE(B6,"/","@",LEN(B6)-LEN(SUBSTITUTE(B6,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/hashicorp/packer/blob/master/LICENSE --output Hashicorp-Packer-LICENSE</v>
+      <c r="H6" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/hashicorp/packer/master/LICENSE --output Hashicorp-Packer-LICENSE</v>
       </c>
     </row>
     <row r="7" spans="1:28" s="39" customFormat="1" ht="15.75" customHeight="1">
@@ -3213,12 +3214,12 @@
       <c r="F7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="82" t="s">
+      <c r="G7" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B7," --output ",SUBSTITUTE(A7," ","-"),"-",IF((LEN(B7)-FIND("@",SUBSTITUTE(B7,"/","@",LEN(B7)-LEN(SUBSTITUTE(B7,"/",""))),1))&gt;0,RIGHT(B7,(LEN(B7)-FIND("@",SUBSTITUTE(B7,"/","@",LEN(B7)-LEN(SUBSTITUTE(B7,"/",""))),1))),SUBSTITUTE(RIGHT(B7,(LEN(B7)-FIND("@",SUBSTITUTE(B7,"/","@",LEN(B7)-LEN(SUBSTITUTE(B7,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/hashicorp/terraform/blob/master/LICENSE --output Hashicorp-Terraform-LICENSE</v>
+      <c r="H7" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/hashicorp/terraform/master/LICENSE --output Hashicorp-Terraform-LICENSE</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="39" customFormat="1" ht="15.75" customHeight="1">
@@ -3238,12 +3239,12 @@
       <c r="F8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="82" t="s">
+      <c r="G8" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B8," --output ",SUBSTITUTE(A8," ","-"),"-",IF((LEN(B8)-FIND("@",SUBSTITUTE(B8,"/","@",LEN(B8)-LEN(SUBSTITUTE(B8,"/",""))),1))&gt;0,RIGHT(B8,(LEN(B8)-FIND("@",SUBSTITUTE(B8,"/","@",LEN(B8)-LEN(SUBSTITUTE(B8,"/",""))),1))),SUBSTITUTE(RIGHT(B8,(LEN(B8)-FIND("@",SUBSTITUTE(B8,"/","@",LEN(B8)-LEN(SUBSTITUTE(B8,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/hashicorp/vault/blob/master/LICENSE --output Hashicorp-Vault-LICENSE</v>
+      <c r="H8" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/hashicorp/vault/master/LICENSE --output Hashicorp-Vault-LICENSE</v>
       </c>
       <c r="J8" s="44"/>
     </row>
@@ -3269,9 +3270,9 @@
       <c r="G9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B9," --output ",SUBSTITUTE(A9," ","-"),"-",IF((LEN(B9)-FIND("@",SUBSTITUTE(B9,"/","@",LEN(B9)-LEN(SUBSTITUTE(B9,"/",""))),1))&gt;0,RIGHT(B9,(LEN(B9)-FIND("@",SUBSTITUTE(B9,"/","@",LEN(B9)-LEN(SUBSTITUTE(B9,"/",""))),1))),SUBSTITUTE(RIGHT(B9,(LEN(B9)-FIND("@",SUBSTITUTE(B9,"/","@",LEN(B9)-LEN(SUBSTITUTE(B9,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/tkem/cachetools/blob/master/LICENSE --output cachetools-LICENSE</v>
+      <c r="H9" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/tkem/cachetools/master/LICENSE --output cachetools-LICENSE</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1">
@@ -3296,9 +3297,9 @@
       <c r="G10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B10," --output ",SUBSTITUTE(A10," ","-"),"-",IF((LEN(B10)-FIND("@",SUBSTITUTE(B10,"/","@",LEN(B10)-LEN(SUBSTITUTE(B10,"/",""))),1))&gt;0,RIGHT(B10,(LEN(B10)-FIND("@",SUBSTITUTE(B10,"/","@",LEN(B10)-LEN(SUBSTITUTE(B10,"/",""))),1))),SUBSTITUTE(RIGHT(B10,(LEN(B10)-FIND("@",SUBSTITUTE(B10,"/","@",LEN(B10)-LEN(SUBSTITUTE(B10,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/GoogleCloudPlatform/google-auth-library-python-httplib2/blob/master/LICENSE --output httplib2-LICENSE</v>
+      <c r="H10" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/GoogleCloudPlatform/google-auth-library-python-httplib2/master/LICENSE --output httplib2-LICENSE</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1">
@@ -3323,9 +3324,9 @@
       <c r="G11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B11," --output ",SUBSTITUTE(A11," ","-"),"-",IF((LEN(B11)-FIND("@",SUBSTITUTE(B11,"/","@",LEN(B11)-LEN(SUBSTITUTE(B11,"/",""))),1))&gt;0,RIGHT(B11,(LEN(B11)-FIND("@",SUBSTITUTE(B11,"/","@",LEN(B11)-LEN(SUBSTITUTE(B11,"/",""))),1))),SUBSTITUTE(RIGHT(B11,(LEN(B11)-FIND("@",SUBSTITUTE(B11,"/","@",LEN(B11)-LEN(SUBSTITUTE(B11,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/beelit94/python-terraform/blob/develop/LICENSE.txt --output python-terraform-LICENSE.txt</v>
+      <c r="H11" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/beelit94/python-terraform/develop/LICENSE.txt --output python-terraform-LICENSE.txt</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1">
@@ -3350,9 +3351,9 @@
       <c r="G12" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B12," --output ",SUBSTITUTE(A12," ","-"),"-",IF((LEN(B12)-FIND("@",SUBSTITUTE(B12,"/","@",LEN(B12)-LEN(SUBSTITUTE(B12,"/",""))),1))&gt;0,RIGHT(B12,(LEN(B12)-FIND("@",SUBSTITUTE(B12,"/","@",LEN(B12)-LEN(SUBSTITUTE(B12,"/",""))),1))),SUBSTITUTE(RIGHT(B12,(LEN(B12)-FIND("@",SUBSTITUTE(B12,"/","@",LEN(B12)-LEN(SUBSTITUTE(B12,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/newvem/pytz/blob/master/LICENSE.txt --output pytz-LICENSE.txt</v>
+      <c r="H12" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/newvem/pytz/master/LICENSE.txt --output pytz-LICENSE.txt</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="12.75">
@@ -3377,9 +3378,9 @@
       <c r="G13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B13," --output ",SUBSTITUTE(A13," ","-"),"-",IF((LEN(B13)-FIND("@",SUBSTITUTE(B13,"/","@",LEN(B13)-LEN(SUBSTITUTE(B13,"/",""))),1))&gt;0,RIGHT(B13,(LEN(B13)-FIND("@",SUBSTITUTE(B13,"/","@",LEN(B13)-LEN(SUBSTITUTE(B13,"/",""))),1))),SUBSTITUTE(RIGHT(B13,(LEN(B13)-FIND("@",SUBSTITUTE(B13,"/","@",LEN(B13)-LEN(SUBSTITUTE(B13,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/yaml/pyyaml/blob/master/LICENSE --output PyYAML-LICENSE</v>
+      <c r="H13" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/yaml/pyyaml/master/LICENSE --output PyYAML-LICENSE</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1">
@@ -3404,9 +3405,9 @@
       <c r="G14" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B14," --output ",SUBSTITUTE(A14," ","-"),"-",IF((LEN(B14)-FIND("@",SUBSTITUTE(B14,"/","@",LEN(B14)-LEN(SUBSTITUTE(B14,"/",""))),1))&gt;0,RIGHT(B14,(LEN(B14)-FIND("@",SUBSTITUTE(B14,"/","@",LEN(B14)-LEN(SUBSTITUTE(B14,"/",""))),1))),SUBSTITUTE(RIGHT(B14,(LEN(B14)-FIND("@",SUBSTITUTE(B14,"/","@",LEN(B14)-LEN(SUBSTITUTE(B14,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/pypa/setuptools/blob/master/LICENSE --output setuptools-LICENSE</v>
+      <c r="H14" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/pypa/setuptools/master/LICENSE --output setuptools-LICENSE</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1">
@@ -3431,9 +3432,9 @@
       <c r="G15" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B15," --output ",SUBSTITUTE(A15," ","-"),"-",IF((LEN(B15)-FIND("@",SUBSTITUTE(B15,"/","@",LEN(B15)-LEN(SUBSTITUTE(B15,"/",""))),1))&gt;0,RIGHT(B15,(LEN(B15)-FIND("@",SUBSTITUTE(B15,"/","@",LEN(B15)-LEN(SUBSTITUTE(B15,"/",""))),1))),SUBSTITUTE(RIGHT(B15,(LEN(B15)-FIND("@",SUBSTITUTE(B15,"/","@",LEN(B15)-LEN(SUBSTITUTE(B15,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/benjaminp/six/blob/master/LICENSE --output six-LICENSE</v>
+      <c r="H15" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/benjaminp/six/master/LICENSE --output six-LICENSE</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1">
@@ -3458,9 +3459,9 @@
       <c r="G16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B16," --output ",SUBSTITUTE(A16," ","-"),"-",IF((LEN(B16)-FIND("@",SUBSTITUTE(B16,"/","@",LEN(B16)-LEN(SUBSTITUTE(B16,"/",""))),1))&gt;0,RIGHT(B16,(LEN(B16)-FIND("@",SUBSTITUTE(B16,"/","@",LEN(B16)-LEN(SUBSTITUTE(B16,"/",""))),1))),SUBSTITUTE(RIGHT(B16,(LEN(B16)-FIND("@",SUBSTITUTE(B16,"/","@",LEN(B16)-LEN(SUBSTITUTE(B16,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/urllib3/urllib3/blob/master/LICENSE.txt --output urllib3-LICENSE.txt</v>
+      <c r="H16" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/urllib3/urllib3/master/LICENSE.txt --output urllib3-LICENSE.txt</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
@@ -3480,12 +3481,12 @@
       <c r="F17" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="82" t="s">
+      <c r="G17" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B17," --output ",SUBSTITUTE(A17," ","-"),"-",IF((LEN(B17)-FIND("@",SUBSTITUTE(B17,"/","@",LEN(B17)-LEN(SUBSTITUTE(B17,"/",""))),1))&gt;0,RIGHT(B17,(LEN(B17)-FIND("@",SUBSTITUTE(B17,"/","@",LEN(B17)-LEN(SUBSTITUTE(B17,"/",""))),1))),SUBSTITUTE(RIGHT(B17,(LEN(B17)-FIND("@",SUBSTITUTE(B17,"/","@",LEN(B17)-LEN(SUBSTITUTE(B17,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/chardet/chardet/blob/master/LICENSE --output chardet-LICENSE</v>
+      <c r="H17" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/chardet/chardet/master/LICENSE --output chardet-LICENSE</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
@@ -3505,11 +3506,11 @@
       <c r="F18" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="82" t="s">
+      <c r="G18" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B18," --output ",SUBSTITUTE(A18," ","-"),"-",IF((LEN(B18)-FIND("@",SUBSTITUTE(B18,"/","@",LEN(B18)-LEN(SUBSTITUTE(B18,"/",""))),1))&gt;0,RIGHT(B18,(LEN(B18)-FIND("@",SUBSTITUTE(B18,"/","@",LEN(B18)-LEN(SUBSTITUTE(B18,"/",""))),1))),SUBSTITUTE(RIGHT(B18,(LEN(B18)-FIND("@",SUBSTITUTE(B18,"/","@",LEN(B18)-LEN(SUBSTITUTE(B18,"/",""))-1),1))),"/","")))</f>
+      <c r="H18" s="55" t="str">
+        <f t="shared" si="0"/>
         <v>curl https://openjdk.java.net/legal/gplv2+ce.html --output OpenJDK8-gplv2+ce.html</v>
       </c>
     </row>
@@ -3535,9 +3536,9 @@
       <c r="G19" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B19," --output ",SUBSTITUTE(A19," ","-"),"-",IF((LEN(B19)-FIND("@",SUBSTITUTE(B19,"/","@",LEN(B19)-LEN(SUBSTITUTE(B19,"/",""))),1))&gt;0,RIGHT(B19,(LEN(B19)-FIND("@",SUBSTITUTE(B19,"/","@",LEN(B19)-LEN(SUBSTITUTE(B19,"/",""))),1))),SUBSTITUTE(RIGHT(B19,(LEN(B19)-FIND("@",SUBSTITUTE(B19,"/","@",LEN(B19)-LEN(SUBSTITUTE(B19,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/kjd/idna/blob/master/LICENSE.rst --output idna-LICENSE.rst</v>
+      <c r="H19" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/kjd/idna/master/LICENSE.rst --output idna-LICENSE.rst</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
@@ -3562,8 +3563,8 @@
       <c r="G20" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B20," --output ",SUBSTITUTE(A20," ","-"),"-",IF((LEN(B20)-FIND("@",SUBSTITUTE(B20,"/","@",LEN(B20)-LEN(SUBSTITUTE(B20,"/",""))),1))&gt;0,RIGHT(B20,(LEN(B20)-FIND("@",SUBSTITUTE(B20,"/","@",LEN(B20)-LEN(SUBSTITUTE(B20,"/",""))),1))),SUBSTITUTE(RIGHT(B20,(LEN(B20)-FIND("@",SUBSTITUTE(B20,"/","@",LEN(B20)-LEN(SUBSTITUTE(B20,"/",""))-1),1))),"/","")))</f>
+      <c r="H20" s="55" t="str">
+        <f t="shared" si="0"/>
         <v>curl http://click.palletsprojects.com/en/5.x/license/ --output Click-license</v>
       </c>
     </row>
@@ -3589,9 +3590,9 @@
       <c r="G21" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B21," --output ",SUBSTITUTE(A21," ","-"),"-",IF((LEN(B21)-FIND("@",SUBSTITUTE(B21,"/","@",LEN(B21)-LEN(SUBSTITUTE(B21,"/",""))),1))&gt;0,RIGHT(B21,(LEN(B21)-FIND("@",SUBSTITUTE(B21,"/","@",LEN(B21)-LEN(SUBSTITUTE(B21,"/",""))),1))),SUBSTITUTE(RIGHT(B21,(LEN(B21)-FIND("@",SUBSTITUTE(B21,"/","@",LEN(B21)-LEN(SUBSTITUTE(B21,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/pallets/flask/blob/master/LICENSE.rst --output Flask-LICENSE.rst</v>
+      <c r="H21" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/pallets/flask/master/LICENSE.rst --output Flask-LICENSE.rst</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
@@ -3616,9 +3617,9 @@
       <c r="G22" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B22," --output ",SUBSTITUTE(A22," ","-"),"-",IF((LEN(B22)-FIND("@",SUBSTITUTE(B22,"/","@",LEN(B22)-LEN(SUBSTITUTE(B22,"/",""))),1))&gt;0,RIGHT(B22,(LEN(B22)-FIND("@",SUBSTITUTE(B22,"/","@",LEN(B22)-LEN(SUBSTITUTE(B22,"/",""))),1))),SUBSTITUTE(RIGHT(B22,(LEN(B22)-FIND("@",SUBSTITUTE(B22,"/","@",LEN(B22)-LEN(SUBSTITUTE(B22,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/gitpython-developers/GitPython/blob/master/LICENSE --output GitPython-LICENSE</v>
+      <c r="H22" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/gitpython-developers/GitPython/master/LICENSE --output GitPython-LICENSE</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
@@ -3643,9 +3644,9 @@
       <c r="G23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B23," --output ",SUBSTITUTE(A23," ","-"),"-",IF((LEN(B23)-FIND("@",SUBSTITUTE(B23,"/","@",LEN(B23)-LEN(SUBSTITUTE(B23,"/",""))),1))&gt;0,RIGHT(B23,(LEN(B23)-FIND("@",SUBSTITUTE(B23,"/","@",LEN(B23)-LEN(SUBSTITUTE(B23,"/",""))),1))),SUBSTITUTE(RIGHT(B23,(LEN(B23)-FIND("@",SUBSTITUTE(B23,"/","@",LEN(B23)-LEN(SUBSTITUTE(B23,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/pallets/itsdangerous/blob/master/LICENSE.rst --output itsdangerous-LICENSE.rst</v>
+      <c r="H23" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/pallets/itsdangerous/master/LICENSE.rst --output itsdangerous-LICENSE.rst</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
@@ -3670,9 +3671,9 @@
       <c r="G24" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B24," --output ",SUBSTITUTE(A24," ","-"),"-",IF((LEN(B24)-FIND("@",SUBSTITUTE(B24,"/","@",LEN(B24)-LEN(SUBSTITUTE(B24,"/",""))),1))&gt;0,RIGHT(B24,(LEN(B24)-FIND("@",SUBSTITUTE(B24,"/","@",LEN(B24)-LEN(SUBSTITUTE(B24,"/",""))),1))),SUBSTITUTE(RIGHT(B24,(LEN(B24)-FIND("@",SUBSTITUTE(B24,"/","@",LEN(B24)-LEN(SUBSTITUTE(B24,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/Kronuz/jinja2/blob/master/LICENSE --output Jinja2-LICENSE</v>
+      <c r="H24" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/Kronuz/jinja2/master/LICENSE --output Jinja2-LICENSE</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
@@ -3697,9 +3698,9 @@
       <c r="G25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B25," --output ",SUBSTITUTE(A25," ","-"),"-",IF((LEN(B25)-FIND("@",SUBSTITUTE(B25,"/","@",LEN(B25)-LEN(SUBSTITUTE(B25,"/",""))),1))&gt;0,RIGHT(B25,(LEN(B25)-FIND("@",SUBSTITUTE(B25,"/","@",LEN(B25)-LEN(SUBSTITUTE(B25,"/",""))),1))),SUBSTITUTE(RIGHT(B25,(LEN(B25)-FIND("@",SUBSTITUTE(B25,"/","@",LEN(B25)-LEN(SUBSTITUTE(B25,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/pallets/markupsafe/blob/master/LICENSE.rst --output MarkupSafe-LICENSE.rst</v>
+      <c r="H25" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/pallets/markupsafe/master/LICENSE.rst --output MarkupSafe-LICENSE.rst</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
@@ -3724,9 +3725,9 @@
       <c r="G26" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B26," --output ",SUBSTITUTE(A26," ","-"),"-",IF((LEN(B26)-FIND("@",SUBSTITUTE(B26,"/","@",LEN(B26)-LEN(SUBSTITUTE(B26,"/",""))),1))&gt;0,RIGHT(B26,(LEN(B26)-FIND("@",SUBSTITUTE(B26,"/","@",LEN(B26)-LEN(SUBSTITUTE(B26,"/",""))),1))),SUBSTITUTE(RIGHT(B26,(LEN(B26)-FIND("@",SUBSTITUTE(B26,"/","@",LEN(B26)-LEN(SUBSTITUTE(B26,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/protocolbuffers/protobuf/blob/master/LICENSE --output protobuf-LICENSE</v>
+      <c r="H26" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/protocolbuffers/protobuf/master/LICENSE --output protobuf-LICENSE</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
@@ -3751,9 +3752,9 @@
       <c r="G27" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B27," --output ",SUBSTITUTE(A27," ","-"),"-",IF((LEN(B27)-FIND("@",SUBSTITUTE(B27,"/","@",LEN(B27)-LEN(SUBSTITUTE(B27,"/",""))),1))&gt;0,RIGHT(B27,(LEN(B27)-FIND("@",SUBSTITUTE(B27,"/","@",LEN(B27)-LEN(SUBSTITUTE(B27,"/",""))),1))),SUBSTITUTE(RIGHT(B27,(LEN(B27)-FIND("@",SUBSTITUTE(B27,"/","@",LEN(B27)-LEN(SUBSTITUTE(B27,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/gitpython-developers/smmap/blob/master/LICENSE --output smmap2-LICENSE</v>
+      <c r="H27" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/gitpython-developers/smmap/master/LICENSE --output smmap2-LICENSE</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
@@ -3778,9 +3779,9 @@
       <c r="G28" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B28," --output ",SUBSTITUTE(A28," ","-"),"-",IF((LEN(B28)-FIND("@",SUBSTITUTE(B28,"/","@",LEN(B28)-LEN(SUBSTITUTE(B28,"/",""))),1))&gt;0,RIGHT(B28,(LEN(B28)-FIND("@",SUBSTITUTE(B28,"/","@",LEN(B28)-LEN(SUBSTITUTE(B28,"/",""))),1))),SUBSTITUTE(RIGHT(B28,(LEN(B28)-FIND("@",SUBSTITUTE(B28,"/","@",LEN(B28)-LEN(SUBSTITUTE(B28,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/uri-templates/uritemplate-py/blob/master/LICENSE --output uritemplate-LICENSE</v>
+      <c r="H28" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/uri-templates/uritemplate-py/master/LICENSE --output uritemplate-LICENSE</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
@@ -3805,9 +3806,9 @@
       <c r="G29" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B29," --output ",SUBSTITUTE(A29," ","-"),"-",IF((LEN(B29)-FIND("@",SUBSTITUTE(B29,"/","@",LEN(B29)-LEN(SUBSTITUTE(B29,"/",""))),1))&gt;0,RIGHT(B29,(LEN(B29)-FIND("@",SUBSTITUTE(B29,"/","@",LEN(B29)-LEN(SUBSTITUTE(B29,"/",""))),1))),SUBSTITUTE(RIGHT(B29,(LEN(B29)-FIND("@",SUBSTITUTE(B29,"/","@",LEN(B29)-LEN(SUBSTITUTE(B29,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/pallets/werkzeug/blob/master/LICENSE.rst --output Werkzeug-LICENSE.rst</v>
+      <c r="H29" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/pallets/werkzeug/master/LICENSE.rst --output Werkzeug-LICENSE.rst</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1">
@@ -3832,9 +3833,9 @@
       <c r="G30" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B30," --output ",SUBSTITUTE(A30," ","-"),"-",IF((LEN(B30)-FIND("@",SUBSTITUTE(B30,"/","@",LEN(B30)-LEN(SUBSTITUTE(B30,"/",""))),1))&gt;0,RIGHT(B30,(LEN(B30)-FIND("@",SUBSTITUTE(B30,"/","@",LEN(B30)-LEN(SUBSTITUTE(B30,"/",""))),1))),SUBSTITUTE(RIGHT(B30,(LEN(B30)-FIND("@",SUBSTITUTE(B30,"/","@",LEN(B30)-LEN(SUBSTITUTE(B30,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/etingof/pyasn1/blob/master/LICENSE.rst --output pyasn1-LICENSE.rst</v>
+      <c r="H30" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/etingof/pyasn1/master/LICENSE.rst --output pyasn1-LICENSE.rst</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1">
@@ -3859,9 +3860,9 @@
       <c r="G31" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B31," --output ",SUBSTITUTE(A31," ","-"),"-",IF((LEN(B31)-FIND("@",SUBSTITUTE(B31,"/","@",LEN(B31)-LEN(SUBSTITUTE(B31,"/",""))),1))&gt;0,RIGHT(B31,(LEN(B31)-FIND("@",SUBSTITUTE(B31,"/","@",LEN(B31)-LEN(SUBSTITUTE(B31,"/",""))),1))),SUBSTITUTE(RIGHT(B31,(LEN(B31)-FIND("@",SUBSTITUTE(B31,"/","@",LEN(B31)-LEN(SUBSTITUTE(B31,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/etingof/pyasn1-modules/blob/master/LICENSE.txt --output pyasn1modules-LICENSE.txt</v>
+      <c r="H31" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/etingof/pyasn1-modules/master/LICENSE.txt --output pyasn1modules-LICENSE.txt</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1">
@@ -3886,9 +3887,9 @@
       <c r="G32" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B32," --output ",SUBSTITUTE(A32," ","-"),"-",IF((LEN(B32)-FIND("@",SUBSTITUTE(B32,"/","@",LEN(B32)-LEN(SUBSTITUTE(B32,"/",""))),1))&gt;0,RIGHT(B32,(LEN(B32)-FIND("@",SUBSTITUTE(B32,"/","@",LEN(B32)-LEN(SUBSTITUTE(B32,"/",""))),1))),SUBSTITUTE(RIGHT(B32,(LEN(B32)-FIND("@",SUBSTITUTE(B32,"/","@",LEN(B32)-LEN(SUBSTITUTE(B32,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/drkjam/netaddr/blob/rel-0.7.x/LICENSE --output netaddr-LICENSE</v>
+      <c r="H32" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/drkjam/netaddr/rel-0.7.x/LICENSE --output netaddr-LICENSE</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1">
@@ -3913,9 +3914,9 @@
       <c r="G33" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H33" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B33," --output ",SUBSTITUTE(A33," ","-"),"-",IF((LEN(B33)-FIND("@",SUBSTITUTE(B33,"/","@",LEN(B33)-LEN(SUBSTITUTE(B33,"/",""))),1))&gt;0,RIGHT(B33,(LEN(B33)-FIND("@",SUBSTITUTE(B33,"/","@",LEN(B33)-LEN(SUBSTITUTE(B33,"/",""))),1))),SUBSTITUTE(RIGHT(B33,(LEN(B33)-FIND("@",SUBSTITUTE(B33,"/","@",LEN(B33)-LEN(SUBSTITUTE(B33,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/gitpython-developers/gitdb/blob/master/LICENSE --output gitdb2-LICENSE</v>
+      <c r="H33" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/gitpython-developers/gitdb/master/LICENSE --output gitdb2-LICENSE</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1">
@@ -3940,8 +3941,8 @@
       <c r="G34" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H34" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B34," --output ",SUBSTITUTE(A34," ","-"),"-",IF((LEN(B34)-FIND("@",SUBSTITUTE(B34,"/","@",LEN(B34)-LEN(SUBSTITUTE(B34,"/",""))),1))&gt;0,RIGHT(B34,(LEN(B34)-FIND("@",SUBSTITUTE(B34,"/","@",LEN(B34)-LEN(SUBSTITUTE(B34,"/",""))),1))),SUBSTITUTE(RIGHT(B34,(LEN(B34)-FIND("@",SUBSTITUTE(B34,"/","@",LEN(B34)-LEN(SUBSTITUTE(B34,"/",""))-1),1))),"/","")))</f>
+      <c r="H34" s="55" t="str">
+        <f t="shared" si="0"/>
         <v>curl https://www.docker.com/legal/components-licenses --output Docker-components-licenses</v>
       </c>
     </row>
@@ -3967,9 +3968,9 @@
       <c r="G35" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H35" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B35," --output ",SUBSTITUTE(A35," ","-"),"-",IF((LEN(B35)-FIND("@",SUBSTITUTE(B35,"/","@",LEN(B35)-LEN(SUBSTITUTE(B35,"/",""))),1))&gt;0,RIGHT(B35,(LEN(B35)-FIND("@",SUBSTITUTE(B35,"/","@",LEN(B35)-LEN(SUBSTITUTE(B35,"/",""))),1))),SUBSTITUTE(RIGHT(B35,(LEN(B35)-FIND("@",SUBSTITUTE(B35,"/","@",LEN(B35)-LEN(SUBSTITUTE(B35,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/googleapis/google-cloud-python/blob/master/LICENSE --output googleapicore-LICENSE</v>
+      <c r="H35" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/googleapis/google-cloud-python/master/LICENSE --output googleapicore-LICENSE</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
@@ -3994,9 +3995,9 @@
       <c r="G36" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B36," --output ",SUBSTITUTE(A36," ","-"),"-",IF((LEN(B36)-FIND("@",SUBSTITUTE(B36,"/","@",LEN(B36)-LEN(SUBSTITUTE(B36,"/",""))),1))&gt;0,RIGHT(B36,(LEN(B36)-FIND("@",SUBSTITUTE(B36,"/","@",LEN(B36)-LEN(SUBSTITUTE(B36,"/",""))),1))),SUBSTITUTE(RIGHT(B36,(LEN(B36)-FIND("@",SUBSTITUTE(B36,"/","@",LEN(B36)-LEN(SUBSTITUTE(B36,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/googleapis/google-api-python-client/blob/master/LICENSE --output googleapipythonclient-LICENSE</v>
+      <c r="H36" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/googleapis/google-api-python-client/master/LICENSE --output googleapipythonclient-LICENSE</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
@@ -4021,9 +4022,9 @@
       <c r="G37" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B37," --output ",SUBSTITUTE(A37," ","-"),"-",IF((LEN(B37)-FIND("@",SUBSTITUTE(B37,"/","@",LEN(B37)-LEN(SUBSTITUTE(B37,"/",""))),1))&gt;0,RIGHT(B37,(LEN(B37)-FIND("@",SUBSTITUTE(B37,"/","@",LEN(B37)-LEN(SUBSTITUTE(B37,"/",""))),1))),SUBSTITUTE(RIGHT(B37,(LEN(B37)-FIND("@",SUBSTITUTE(B37,"/","@",LEN(B37)-LEN(SUBSTITUTE(B37,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/googleapis/googleapis/blob/master/LICENSE --output googleapiscommonprotos-LICENSE</v>
+      <c r="H37" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/googleapis/googleapis/master/LICENSE --output googleapiscommonprotos-LICENSE</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
@@ -4048,9 +4049,9 @@
       <c r="G38" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B38," --output ",SUBSTITUTE(A38," ","-"),"-",IF((LEN(B38)-FIND("@",SUBSTITUTE(B38,"/","@",LEN(B38)-LEN(SUBSTITUTE(B38,"/",""))),1))&gt;0,RIGHT(B38,(LEN(B38)-FIND("@",SUBSTITUTE(B38,"/","@",LEN(B38)-LEN(SUBSTITUTE(B38,"/",""))),1))),SUBSTITUTE(RIGHT(B38,(LEN(B38)-FIND("@",SUBSTITUTE(B38,"/","@",LEN(B38)-LEN(SUBSTITUTE(B38,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/googleapis/google-auth-library-python/blob/master/LICENSE --output googleauth-LICENSE</v>
+      <c r="H38" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/googleapis/google-auth-library-python/master/LICENSE --output googleauth-LICENSE</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
@@ -4075,9 +4076,9 @@
       <c r="G39" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B39," --output ",SUBSTITUTE(A39," ","-"),"-",IF((LEN(B39)-FIND("@",SUBSTITUTE(B39,"/","@",LEN(B39)-LEN(SUBSTITUTE(B39,"/",""))),1))&gt;0,RIGHT(B39,(LEN(B39)-FIND("@",SUBSTITUTE(B39,"/","@",LEN(B39)-LEN(SUBSTITUTE(B39,"/",""))),1))),SUBSTITUTE(RIGHT(B39,(LEN(B39)-FIND("@",SUBSTITUTE(B39,"/","@",LEN(B39)-LEN(SUBSTITUTE(B39,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/googleapis/google-cloud-python/blob/master/LICENSE --output googlecloudcore-LICENSE</v>
+      <c r="H39" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/googleapis/google-cloud-python/master/LICENSE --output googlecloudcore-LICENSE</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1">
@@ -4102,9 +4103,9 @@
       <c r="G40" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H40" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B40," --output ",SUBSTITUTE(A40," ","-"),"-",IF((LEN(B40)-FIND("@",SUBSTITUTE(B40,"/","@",LEN(B40)-LEN(SUBSTITUTE(B40,"/",""))),1))&gt;0,RIGHT(B40,(LEN(B40)-FIND("@",SUBSTITUTE(B40,"/","@",LEN(B40)-LEN(SUBSTITUTE(B40,"/",""))),1))),SUBSTITUTE(RIGHT(B40,(LEN(B40)-FIND("@",SUBSTITUTE(B40,"/","@",LEN(B40)-LEN(SUBSTITUTE(B40,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/GoogleCloudPlatform/google-cloud-datastore/blob/master/LICENSE --output googleclouddatastore-LICENSE</v>
+      <c r="H40" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/GoogleCloudPlatform/google-cloud-datastore/master/LICENSE --output googleclouddatastore-LICENSE</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1">
@@ -4129,9 +4130,9 @@
       <c r="G41" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H41" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B41," --output ",SUBSTITUTE(A41," ","-"),"-",IF((LEN(B41)-FIND("@",SUBSTITUTE(B41,"/","@",LEN(B41)-LEN(SUBSTITUTE(B41,"/",""))),1))&gt;0,RIGHT(B41,(LEN(B41)-FIND("@",SUBSTITUTE(B41,"/","@",LEN(B41)-LEN(SUBSTITUTE(B41,"/",""))),1))),SUBSTITUTE(RIGHT(B41,(LEN(B41)-FIND("@",SUBSTITUTE(B41,"/","@",LEN(B41)-LEN(SUBSTITUTE(B41,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/helm/helm/blob/master/LICENSE --output Helm-LICENSE</v>
+      <c r="H41" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/helm/helm/master/LICENSE --output Helm-LICENSE</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1">
@@ -4156,9 +4157,9 @@
       <c r="G42" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H42" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B42," --output ",SUBSTITUTE(A42," ","-"),"-",IF((LEN(B42)-FIND("@",SUBSTITUTE(B42,"/","@",LEN(B42)-LEN(SUBSTITUTE(B42,"/",""))),1))&gt;0,RIGHT(B42,(LEN(B42)-FIND("@",SUBSTITUTE(B42,"/","@",LEN(B42)-LEN(SUBSTITUTE(B42,"/",""))),1))),SUBSTITUTE(RIGHT(B42,(LEN(B42)-FIND("@",SUBSTITUTE(B42,"/","@",LEN(B42)-LEN(SUBSTITUTE(B42,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/istio/istio/blob/master/LICENSE --output Istio-LICENSE</v>
+      <c r="H42" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/istio/istio/master/LICENSE --output Istio-LICENSE</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1">
@@ -4183,9 +4184,9 @@
       <c r="G43" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B43," --output ",SUBSTITUTE(A43," ","-"),"-",IF((LEN(B43)-FIND("@",SUBSTITUTE(B43,"/","@",LEN(B43)-LEN(SUBSTITUTE(B43,"/",""))),1))&gt;0,RIGHT(B43,(LEN(B43)-FIND("@",SUBSTITUTE(B43,"/","@",LEN(B43)-LEN(SUBSTITUTE(B43,"/",""))),1))),SUBSTITUTE(RIGHT(B43,(LEN(B43)-FIND("@",SUBSTITUTE(B43,"/","@",LEN(B43)-LEN(SUBSTITUTE(B43,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/kubernetes/kubernetes/blob/master/LICENSE --output Kubernetes-LICENSE</v>
+      <c r="H43" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/kubernetes/kubernetes/master/LICENSE --output Kubernetes-LICENSE</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
@@ -4210,9 +4211,9 @@
       <c r="G44" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H44" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B44," --output ",SUBSTITUTE(A44," ","-"),"-",IF((LEN(B44)-FIND("@",SUBSTITUTE(B44,"/","@",LEN(B44)-LEN(SUBSTITUTE(B44,"/",""))),1))&gt;0,RIGHT(B44,(LEN(B44)-FIND("@",SUBSTITUTE(B44,"/","@",LEN(B44)-LEN(SUBSTITUTE(B44,"/",""))),1))),SUBSTITUTE(RIGHT(B44,(LEN(B44)-FIND("@",SUBSTITUTE(B44,"/","@",LEN(B44)-LEN(SUBSTITUTE(B44,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/googleapis/oauth2client/blob/master/LICENSE --output oauth2client-LICENSE</v>
+      <c r="H44" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/googleapis/oauth2client/master/LICENSE --output oauth2client-LICENSE</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
@@ -4237,9 +4238,9 @@
       <c r="G45" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H45" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B45," --output ",SUBSTITUTE(A45," ","-"),"-",IF((LEN(B45)-FIND("@",SUBSTITUTE(B45,"/","@",LEN(B45)-LEN(SUBSTITUTE(B45,"/",""))),1))&gt;0,RIGHT(B45,(LEN(B45)-FIND("@",SUBSTITUTE(B45,"/","@",LEN(B45)-LEN(SUBSTITUTE(B45,"/",""))),1))),SUBSTITUTE(RIGHT(B45,(LEN(B45)-FIND("@",SUBSTITUTE(B45,"/","@",LEN(B45)-LEN(SUBSTITUTE(B45,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/prometheus/prometheus/blob/master/LICENSE --output Prometheus-LICENSE</v>
+      <c r="H45" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/prometheus/prometheus/master/LICENSE --output Prometheus-LICENSE</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1">
@@ -4264,9 +4265,9 @@
       <c r="G46" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H46" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B46," --output ",SUBSTITUTE(A46," ","-"),"-",IF((LEN(B46)-FIND("@",SUBSTITUTE(B46,"/","@",LEN(B46)-LEN(SUBSTITUTE(B46,"/",""))),1))&gt;0,RIGHT(B46,(LEN(B46)-FIND("@",SUBSTITUTE(B46,"/","@",LEN(B46)-LEN(SUBSTITUTE(B46,"/",""))),1))),SUBSTITUTE(RIGHT(B46,(LEN(B46)-FIND("@",SUBSTITUTE(B46,"/","@",LEN(B46)-LEN(SUBSTITUTE(B46,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/psf/requests/blob/master/LICENSE --output requests-LICENSE</v>
+      <c r="H46" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>curl https://raw.githubusercontent.com/psf/requests/master/LICENSE --output requests-LICENSE</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1">
@@ -4291,9 +4292,9 @@
       <c r="G47" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H47" s="44" t="str">
-        <f>_xlfn.CONCAT("curl ",B47," --output ",SUBSTITUTE(A47," ","-"),"-",IF((LEN(B47)-FIND("@",SUBSTITUTE(B47,"/","@",LEN(B47)-LEN(SUBSTITUTE(B47,"/",""))),1))&gt;0,RIGHT(B47,(LEN(B47)-FIND("@",SUBSTITUTE(B47,"/","@",LEN(B47)-LEN(SUBSTITUTE(B47,"/",""))),1))),SUBSTITUTE(RIGHT(B47,(LEN(B47)-FIND("@",SUBSTITUTE(B47,"/","@",LEN(B47)-LEN(SUBSTITUTE(B47,"/",""))-1),1))),"/","")))</f>
-        <v>curl https://github.com/sybrenstuvel/python-rsa/blob/master/LICENSE --output rsa-LICENSE</v>
+      <c r="H47" s="55" t="str">
+        <f>_xlfn.CONCAT("curl ",SUBSTITUTE(SUBSTITUTE(B47,"github.com","raw.githubusercontent.com"),"/blob","")," --output ",SUBSTITUTE(A47," ","-"),"-",IF((LEN(B47)-FIND("@",SUBSTITUTE(B47,"/","@",LEN(B47)-LEN(SUBSTITUTE(B47,"/",""))),1))&gt;0,RIGHT(B47,(LEN(B47)-FIND("@",SUBSTITUTE(B47,"/","@",LEN(B47)-LEN(SUBSTITUTE(B47,"/",""))),1))),SUBSTITUTE(RIGHT(B47,(LEN(B47)-FIND("@",SUBSTITUTE(B47,"/","@",LEN(B47)-LEN(SUBSTITUTE(B47,"/",""))-1),1))),"/","")))</f>
+        <v>curl https://raw.githubusercontent.com/sybrenstuvel/python-rsa/master/LICENSE --output rsa-LICENSE</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
@@ -7874,7 +7875,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="H4:K5"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -7888,14 +7889,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
       <c r="I1" s="24"/>
@@ -7905,31 +7906,31 @@
       <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
       <c r="G2" s="26"/>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" ht="38.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
       <c r="G3" s="26"/>
       <c r="H3" s="27" t="s">
         <v>33</v>
@@ -7947,12 +7948,12 @@
       <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:13" ht="25.5">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
       <c r="G4" s="26"/>
       <c r="H4" s="27" t="s">
         <v>39</v>
@@ -7970,12 +7971,12 @@
       <c r="M4" s="24"/>
     </row>
     <row r="5" spans="1:13" ht="38.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
       <c r="G5" s="26"/>
       <c r="H5" s="27" t="s">
         <v>43</v>
@@ -7993,12 +7994,12 @@
       <c r="M5" s="24"/>
     </row>
     <row r="6" spans="1:13" ht="25.5">
-      <c r="A6" s="64"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="26"/>
       <c r="H6" s="27" t="s">
         <v>45</v>
@@ -8016,12 +8017,12 @@
       <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:13" ht="76.5">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="26"/>
       <c r="H7" s="27" t="s">
         <v>47</v>
@@ -8042,19 +8043,19 @@
       <c r="A8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="74" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
@@ -8063,253 +8064,253 @@
       <c r="A9" s="34">
         <v>1</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="78" t="s">
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="60"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="63"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="35">
         <v>2</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="69" t="s">
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="58"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="35">
         <v>3</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="69" t="s">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="58"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="61"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="35">
         <v>4</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="77" t="s">
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="58"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="61"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="35">
         <v>5</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="69" t="s">
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="58"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="61"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="35">
         <v>6</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="69" t="s">
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="58"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="61"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="35">
         <v>7</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="79" t="s">
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="58"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="61"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="35">
         <v>8</v>
       </c>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="69" t="s">
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="58"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="61"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="35">
         <v>9</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="69" t="s">
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="58"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="61"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="35">
         <v>10</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="69" t="s">
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="58"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="61"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="35">
         <v>11</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="69" t="s">
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="58"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="61"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="36">
         <v>12</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="70" t="s">
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="56"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -8353,7 +8354,7 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -8374,7 +8375,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added git screenshots where users can find OSS license texts and source code (where applies)
</commit_message>
<xml_diff>
--- a/tb-oss/Open Source Compliance Worksheet.xlsx
+++ b/tb-oss/Open Source Compliance Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orme\tranquility-base\tb-oss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orme\tranquility-base\tb-gcp\tb-oss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D441D2B-5DC7-4C2B-8F4E-E3D62E023BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7144A5C9-BA82-4FC2-801B-A8078DACCAA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3825" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions and introduction" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -1260,7 +1262,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1275,19 +1290,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1306,6 +1308,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10066</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{294DDA4D-C28F-4D92-8BBC-11D97257B6D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6229350" y="0"/>
+          <a:ext cx="5991766" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>45145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1DE97F9-F57E-4BDD-88AF-7ABC1C7FF1AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11249025" y="2066925"/>
+          <a:ext cx="10058400" cy="5855395"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3031,7 +3138,7 @@
   </sheetPr>
   <dimension ref="A1:AB996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -6836,8 +6943,8 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7863,6 +7970,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7889,7 +7997,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="79" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="67"/>
@@ -7906,7 +8014,7 @@
       <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="80" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="67"/>
@@ -7915,7 +8023,7 @@
       <c r="E2" s="67"/>
       <c r="F2" s="67"/>
       <c r="G2" s="26"/>
-      <c r="H2" s="76" t="s">
+      <c r="H2" s="81" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="71"/>
@@ -8043,12 +8151,12 @@
       <c r="A8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="82" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="67"/>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="82" t="s">
         <v>51</v>
       </c>
       <c r="F8" s="67"/>
@@ -8064,33 +8172,33 @@
       <c r="A9" s="34">
         <v>1</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="81" t="s">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
       <c r="M9" s="63"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="35">
         <v>2</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="75" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="67"/>
       <c r="D10" s="67"/>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="75" t="s">
         <v>55</v>
       </c>
       <c r="F10" s="67"/>
@@ -8106,12 +8214,12 @@
       <c r="A11" s="35">
         <v>3</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="74" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="67"/>
       <c r="D11" s="67"/>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="75" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="67"/>
@@ -8127,12 +8235,12 @@
       <c r="A12" s="35">
         <v>4</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="77" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="67"/>
       <c r="D12" s="67"/>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="74" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="67"/>
@@ -8148,12 +8256,12 @@
       <c r="A13" s="35">
         <v>5</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="74" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13" s="67"/>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="75" t="s">
         <v>61</v>
       </c>
       <c r="F13" s="67"/>
@@ -8169,12 +8277,12 @@
       <c r="A14" s="35">
         <v>6</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="75" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="67"/>
       <c r="D14" s="67"/>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="75" t="s">
         <v>63</v>
       </c>
       <c r="F14" s="67"/>
@@ -8190,12 +8298,12 @@
       <c r="A15" s="35">
         <v>7</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="74" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="67"/>
       <c r="D15" s="67"/>
-      <c r="E15" s="82" t="s">
+      <c r="E15" s="76" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="67"/>
@@ -8211,12 +8319,12 @@
       <c r="A16" s="35">
         <v>8</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="75" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="67"/>
       <c r="D16" s="67"/>
-      <c r="E16" s="72" t="s">
+      <c r="E16" s="75" t="s">
         <v>67</v>
       </c>
       <c r="F16" s="67"/>
@@ -8232,12 +8340,12 @@
       <c r="A17" s="35">
         <v>9</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="75" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="67"/>
       <c r="D17" s="67"/>
-      <c r="E17" s="72" t="s">
+      <c r="E17" s="75" t="s">
         <v>69</v>
       </c>
       <c r="F17" s="67"/>
@@ -8253,12 +8361,12 @@
       <c r="A18" s="35">
         <v>10</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="75" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="67"/>
       <c r="D18" s="67"/>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="75" t="s">
         <v>71</v>
       </c>
       <c r="F18" s="67"/>
@@ -8274,12 +8382,12 @@
       <c r="A19" s="35">
         <v>11</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="75" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="67"/>
       <c r="D19" s="67"/>
-      <c r="E19" s="72" t="s">
+      <c r="E19" s="75" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="67"/>
@@ -8295,12 +8403,12 @@
       <c r="A20" s="36">
         <v>12</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="78" t="s">
         <v>74</v>
       </c>
       <c r="C20" s="71"/>
       <c r="D20" s="71"/>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="78" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="71"/>
@@ -8314,19 +8422,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="E12:M12"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E15:M15"/>
-    <mergeCell ref="E16:M16"/>
-    <mergeCell ref="E17:M17"/>
-    <mergeCell ref="E18:M18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:M19"/>
     <mergeCell ref="E20:M20"/>
@@ -8343,6 +8438,19 @@
     <mergeCell ref="E11:M11"/>
     <mergeCell ref="E14:M14"/>
     <mergeCell ref="E13:M13"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E18:M18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added git screenshots where users can find OSS license texts and source code (where applies) (#130)
</commit_message>
<xml_diff>
--- a/tb-oss/Open Source Compliance Worksheet.xlsx
+++ b/tb-oss/Open Source Compliance Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orme\tranquility-base\tb-oss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orme\tranquility-base\tb-gcp\tb-oss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D441D2B-5DC7-4C2B-8F4E-E3D62E023BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7144A5C9-BA82-4FC2-801B-A8078DACCAA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3825" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions and introduction" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -1260,7 +1262,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1275,19 +1290,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1306,6 +1308,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10066</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{294DDA4D-C28F-4D92-8BBC-11D97257B6D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6229350" y="0"/>
+          <a:ext cx="5991766" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>45145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1DE97F9-F57E-4BDD-88AF-7ABC1C7FF1AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11249025" y="2066925"/>
+          <a:ext cx="10058400" cy="5855395"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3031,7 +3138,7 @@
   </sheetPr>
   <dimension ref="A1:AB996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -6836,8 +6943,8 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7863,6 +7970,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7889,7 +7997,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="79" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="67"/>
@@ -7906,7 +8014,7 @@
       <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="80" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="67"/>
@@ -7915,7 +8023,7 @@
       <c r="E2" s="67"/>
       <c r="F2" s="67"/>
       <c r="G2" s="26"/>
-      <c r="H2" s="76" t="s">
+      <c r="H2" s="81" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="71"/>
@@ -8043,12 +8151,12 @@
       <c r="A8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="82" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="67"/>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="82" t="s">
         <v>51</v>
       </c>
       <c r="F8" s="67"/>
@@ -8064,33 +8172,33 @@
       <c r="A9" s="34">
         <v>1</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="81" t="s">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
       <c r="M9" s="63"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="35">
         <v>2</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="75" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="67"/>
       <c r="D10" s="67"/>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="75" t="s">
         <v>55</v>
       </c>
       <c r="F10" s="67"/>
@@ -8106,12 +8214,12 @@
       <c r="A11" s="35">
         <v>3</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="74" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="67"/>
       <c r="D11" s="67"/>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="75" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="67"/>
@@ -8127,12 +8235,12 @@
       <c r="A12" s="35">
         <v>4</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="77" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="67"/>
       <c r="D12" s="67"/>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="74" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="67"/>
@@ -8148,12 +8256,12 @@
       <c r="A13" s="35">
         <v>5</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="74" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13" s="67"/>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="75" t="s">
         <v>61</v>
       </c>
       <c r="F13" s="67"/>
@@ -8169,12 +8277,12 @@
       <c r="A14" s="35">
         <v>6</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="75" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="67"/>
       <c r="D14" s="67"/>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="75" t="s">
         <v>63</v>
       </c>
       <c r="F14" s="67"/>
@@ -8190,12 +8298,12 @@
       <c r="A15" s="35">
         <v>7</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="74" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="67"/>
       <c r="D15" s="67"/>
-      <c r="E15" s="82" t="s">
+      <c r="E15" s="76" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="67"/>
@@ -8211,12 +8319,12 @@
       <c r="A16" s="35">
         <v>8</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="75" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="67"/>
       <c r="D16" s="67"/>
-      <c r="E16" s="72" t="s">
+      <c r="E16" s="75" t="s">
         <v>67</v>
       </c>
       <c r="F16" s="67"/>
@@ -8232,12 +8340,12 @@
       <c r="A17" s="35">
         <v>9</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="75" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="67"/>
       <c r="D17" s="67"/>
-      <c r="E17" s="72" t="s">
+      <c r="E17" s="75" t="s">
         <v>69</v>
       </c>
       <c r="F17" s="67"/>
@@ -8253,12 +8361,12 @@
       <c r="A18" s="35">
         <v>10</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="75" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="67"/>
       <c r="D18" s="67"/>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="75" t="s">
         <v>71</v>
       </c>
       <c r="F18" s="67"/>
@@ -8274,12 +8382,12 @@
       <c r="A19" s="35">
         <v>11</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="75" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="67"/>
       <c r="D19" s="67"/>
-      <c r="E19" s="72" t="s">
+      <c r="E19" s="75" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="67"/>
@@ -8295,12 +8403,12 @@
       <c r="A20" s="36">
         <v>12</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="78" t="s">
         <v>74</v>
       </c>
       <c r="C20" s="71"/>
       <c r="D20" s="71"/>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="78" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="71"/>
@@ -8314,19 +8422,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="E12:M12"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E15:M15"/>
-    <mergeCell ref="E16:M16"/>
-    <mergeCell ref="E17:M17"/>
-    <mergeCell ref="E18:M18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:M19"/>
     <mergeCell ref="E20:M20"/>
@@ -8343,6 +8438,19 @@
     <mergeCell ref="E11:M11"/>
     <mergeCell ref="E14:M14"/>
     <mergeCell ref="E13:M13"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E18:M18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>